<commit_message>
updated story board planning to what makes sense in my head. - Added correct mapping to site.css
</commit_message>
<xml_diff>
--- a/Documents/Story_Board.xlsx
+++ b/Documents/Story_Board.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vazqu\Cloud\School\Stevens\web_programming\Web_Programming_Final_Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8555B828-E1CF-4B0A-9363-74089FF5F59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E3B6BD-34F5-4D22-B1B2-E62C6B0E1532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15990" xr2:uid="{CBA8CBC5-113E-4324-A52E-B53175C52534}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13692" activeTab="2" xr2:uid="{CBA8CBC5-113E-4324-A52E-B53175C52534}"/>
   </bookViews>
   <sheets>
     <sheet name="Story1" sheetId="1" r:id="rId1"/>
     <sheet name="Story2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -344,6 +345,115 @@
   </si>
   <si>
     <t>click on selected page button should direct user to that page</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Posts</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Design GUI</t>
+  </si>
+  <si>
+    <t>Authenticate in middleware</t>
+  </si>
+  <si>
+    <t>Add user to database</t>
+  </si>
+  <si>
+    <t>Add post</t>
+  </si>
+  <si>
+    <t>Remove post</t>
+  </si>
+  <si>
+    <t>Update post upvotes</t>
+  </si>
+  <si>
+    <t>Add event</t>
+  </si>
+  <si>
+    <t>Update event</t>
+  </si>
+  <si>
+    <t>Remove event</t>
+  </si>
+  <si>
+    <t>View word frequency breakdown</t>
+  </si>
+  <si>
+    <t>Requires</t>
+  </si>
+  <si>
+    <t>- Middleware to create and add user to session. 
+- Middleware to check if user logged in, redirect to posts if so</t>
+  </si>
+  <si>
+    <t>- section for user to enter username
+- section for user to enter password
+- section for user to enter confirmation password
+- register button to post data
+- main navigation link
+- navigation link to Registration page</t>
+  </si>
+  <si>
+    <t>- section for user to enter username
+- section for user to enter password
+- login button to post data
+- main navigation link
+- navigation link to Registration page</t>
+  </si>
+  <si>
+    <t>- Register button click should post data to /register route
+- /register POST route should validate and add user to database, if successful, return user to login page with success message. Otherwise return error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- section to POST post
+   - Should contain post title entry section
+   - Should contain post content entry section
+  - should contain post button
+-section to GET posts
+   - Post should contain username, userid, date and time, post content, post title, number of upvotes for post, word breakdown button, comment section for post
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- POST updated post; adding/removing userID from post upvote userId list when user toggles checkbox </t>
+  </si>
+  <si>
+    <t>*** Didn't put in requirements, add if time allows</t>
+  </si>
+  <si>
+    <t>- Displays word breakdown
+- Should just have a GET route to display posts breakdown</t>
+  </si>
+  <si>
+    <t>- Submit post button click should POST data to posts route and update the database with post data</t>
+  </si>
+  <si>
+    <t>- section to POST event
+   - should contain fields to insert event event name, event location, date, time, description, upload button to upload banner image, and a create event button
+- section to GET events
+   - should contain event event name, event location, date, time, description, banner image</t>
+  </si>
+  <si>
+    <t>- POST route for events should validate event and add to database</t>
+  </si>
+  <si>
+    <t>* Note POST references the HTTP method, while Post/post refer to the content a user can create and view
+* Anything not required should be looked into last</t>
+  </si>
+  <si>
+    <t>***NOT REQUIREMENT</t>
   </si>
 </sst>
 </file>
@@ -415,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -438,6 +548,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0B601E-78EB-40C7-9FCF-21B6D3D04076}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,16 +883,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1006,4 +1122,191 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9922CF68-4136-4E38-8D95-94BA8FA8C07E}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="89.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>